<commit_message>
Updated R1 to 910 ohms.
</commit_message>
<xml_diff>
--- a/PCB/harp timestamp generator gen1 BOM.xlsx
+++ b/PCB/harp timestamp generator gen1 BOM.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23530"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\My Drive\_filipe\harp clock generator v1.0\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\OEPS\Documents\github\harp-tech\harp_timestamp_generator_Gen1\PCB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E564F6C9-2B97-4133-A72F-E72C774EC144}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59EA7DEB-5421-4CA2-98E2-AE9342B4676C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1680" yWindow="3270" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="harp expander v1" sheetId="1" r:id="rId1"/>
@@ -165,15 +165,6 @@
     <t>EMK107BBJ106MA-T</t>
   </si>
   <si>
-    <t>RK73B1ETTP331J</t>
-  </si>
-  <si>
-    <t>2019-RK73B1ETTP331JDKR-ND</t>
-  </si>
-  <si>
-    <t>330 1/10W 5%</t>
-  </si>
-  <si>
     <t>10uF 16V X5R 10%</t>
   </si>
   <si>
@@ -196,6 +187,15 @@
   </si>
   <si>
     <t>Farnell</t>
+  </si>
+  <si>
+    <t>RK73B1ETTP911J</t>
+  </si>
+  <si>
+    <t>2019-RK73B1ETTP911JDKR-ND</t>
+  </si>
+  <si>
+    <t>910 1/10W 5%</t>
   </si>
 </sst>
 </file>
@@ -1122,7 +1122,7 @@
   <dimension ref="A1:H17"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13:H13"/>
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1180,7 +1180,7 @@
         <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="C3" t="s">
         <v>5</v>
@@ -1198,7 +1198,7 @@
         <v>30</v>
       </c>
       <c r="H3" s="6" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -1206,7 +1206,7 @@
         <v>1</v>
       </c>
       <c r="B4" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="C4" t="s">
         <v>8</v>
@@ -1224,7 +1224,7 @@
         <v>30</v>
       </c>
       <c r="H4" s="6" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -1232,7 +1232,7 @@
         <v>1</v>
       </c>
       <c r="B5" t="s">
-        <v>45</v>
+        <v>53</v>
       </c>
       <c r="C5" t="s">
         <v>6</v>
@@ -1241,7 +1241,7 @@
         <v>7</v>
       </c>
       <c r="E5" t="s">
-        <v>43</v>
+        <v>51</v>
       </c>
       <c r="F5" s="7" t="s">
         <v>17</v>
@@ -1250,7 +1250,7 @@
         <v>30</v>
       </c>
       <c r="H5" t="s">
-        <v>44</v>
+        <v>52</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
@@ -1267,7 +1267,7 @@
         <v>26</v>
       </c>
       <c r="E6" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="F6" s="7" t="s">
         <v>17</v>
@@ -1276,7 +1276,7 @@
         <v>30</v>
       </c>
       <c r="H6" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
@@ -1328,7 +1328,7 @@
         <v>30</v>
       </c>
       <c r="H8" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
@@ -1392,7 +1392,7 @@
         <v>12</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="H13">
         <v>3712278</v>

</xml_diff>

<commit_message>
Corrected the PN of the audio cable.
</commit_message>
<xml_diff>
--- a/PCB/harp timestamp generator gen1 BOM.xlsx
+++ b/PCB/harp timestamp generator gen1 BOM.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\OEPS\Documents\github\harp-tech\harp_timestamp_generator_Gen1\PCB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59EA7DEB-5421-4CA2-98E2-AE9342B4676C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FE19EC1-6C03-4852-93F7-7B350DE8FE60}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="harp expander v1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="54">
   <si>
     <t>Qty</t>
   </si>
@@ -72,9 +72,6 @@
     <t>3.5mm stereo jack cable 0.3 m, Black</t>
   </si>
   <si>
-    <t>AV13646</t>
-  </si>
-  <si>
     <t>Number of unique parts</t>
   </si>
   <si>
@@ -186,9 +183,6 @@
     <t>5975004407F</t>
   </si>
   <si>
-    <t>Farnell</t>
-  </si>
-  <si>
     <t>RK73B1ETTP911J</t>
   </si>
   <si>
@@ -196,6 +190,12 @@
   </si>
   <si>
     <t>910 1/10W 5%</t>
+  </si>
+  <si>
+    <t>TL1621-ND</t>
+  </si>
+  <si>
+    <t>P312-001</t>
   </si>
 </sst>
 </file>
@@ -1122,7 +1122,7 @@
   <dimension ref="A1:H17"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+      <selection activeCell="H23" sqref="H23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1154,18 +1154,18 @@
         <v>4</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G1" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="H1" s="3" t="s">
         <v>33</v>
-      </c>
-      <c r="H1" s="3" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B2" s="8"/>
       <c r="C2" s="8"/>
@@ -1180,25 +1180,25 @@
         <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C3" t="s">
         <v>5</v>
       </c>
       <c r="D3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E3" s="6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F3" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G3" s="7" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H3" s="6" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -1206,25 +1206,25 @@
         <v>1</v>
       </c>
       <c r="B4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C4" t="s">
         <v>8</v>
       </c>
       <c r="D4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F4" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G4" s="7" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H4" s="6" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -1232,7 +1232,7 @@
         <v>1</v>
       </c>
       <c r="B5" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C5" t="s">
         <v>6</v>
@@ -1241,16 +1241,16 @@
         <v>7</v>
       </c>
       <c r="E5" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G5" s="7" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H5" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
@@ -1258,25 +1258,25 @@
         <v>1</v>
       </c>
       <c r="B6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C6" t="s">
         <v>24</v>
       </c>
-      <c r="C6" t="s">
+      <c r="D6" t="s">
         <v>25</v>
       </c>
-      <c r="D6" t="s">
-        <v>26</v>
-      </c>
       <c r="E6" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F6" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G6" s="7" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
@@ -1284,25 +1284,25 @@
         <v>1</v>
       </c>
       <c r="B7" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C7" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D7" t="s">
         <v>10</v>
       </c>
       <c r="E7" t="s">
+        <v>35</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G7" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="H7" t="s">
         <v>36</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="G7" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="H7" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
@@ -1310,25 +1310,25 @@
         <v>1</v>
       </c>
       <c r="B8" t="s">
+        <v>37</v>
+      </c>
+      <c r="C8" t="s">
         <v>38</v>
       </c>
-      <c r="C8" t="s">
-        <v>39</v>
-      </c>
       <c r="D8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E8" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G8" s="7" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H8" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
@@ -1336,27 +1336,27 @@
         <v>1</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D9" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E9" s="6" t="s">
         <v>9</v>
       </c>
       <c r="F9" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G9" s="7" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H9" s="6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B10" s="8"/>
       <c r="C10" s="8"/>
@@ -1371,7 +1371,7 @@
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="8" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B12" s="8"/>
       <c r="C12" s="8"/>
@@ -1389,18 +1389,18 @@
         <v>11</v>
       </c>
       <c r="E13" t="s">
-        <v>12</v>
-      </c>
-      <c r="G13" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="H13">
-        <v>3712278</v>
+        <v>53</v>
+      </c>
+      <c r="G13" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="H13" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="8" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B14" s="8"/>
       <c r="C14" s="8"/>
@@ -1412,7 +1412,7 @@
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="E15" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F15" s="1">
         <v>7</v>
@@ -1420,7 +1420,7 @@
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="E16" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F16" s="1">
         <v>10</v>
@@ -1428,7 +1428,7 @@
     </row>
     <row r="17" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E17" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F17" s="1">
         <v>0</v>

</xml_diff>